<commit_message>
PowerPack - Hidros Part List Update
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/data/programDatabase/Hidrolik2.xlsx
+++ b/src/main/resources/assets/data/programDatabase/Hidrolik2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hidirektor/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hidirektor/IdeaProjects/ondergrup-hydraulic-tool/src/main/resources/assets/data/programDatabase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91E81AB-7BCD-EB45-ADF5-7B8A916A443B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11B5E8C-A79F-BB4E-AD15-6B50FC374556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="28480" windowHeight="15500" tabRatio="897" firstSheet="43" activeTab="43" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="28480" windowHeight="15500" tabRatio="897" firstSheet="48" activeTab="49" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kabinler" sheetId="55" r:id="rId1"/>
@@ -48,30 +48,30 @@
     <sheet name="Hidros-Platform" sheetId="30" r:id="rId33"/>
     <sheet name="Hidros-Valf-Deger" sheetId="31" r:id="rId34"/>
     <sheet name="Parça-Hidros-Motor380" sheetId="32" r:id="rId35"/>
-    <sheet name="Parça-İthal-Motor380" sheetId="66" r:id="rId36"/>
-    <sheet name="Parça-Hidros-Motor220" sheetId="33" r:id="rId37"/>
+    <sheet name="Parça-Hidros-Motor220" sheetId="33" r:id="rId36"/>
+    <sheet name="Parça-İthal-Motor380" sheetId="66" r:id="rId37"/>
     <sheet name="Parça-İthal-Motor220" sheetId="67" r:id="rId38"/>
     <sheet name="Parça-Hidros-Pompa" sheetId="34" r:id="rId39"/>
-    <sheet name="Parça-İthal-Pompa" sheetId="68" r:id="rId40"/>
-    <sheet name="Parça-Hidros-Pompa-Civata" sheetId="35" r:id="rId41"/>
-    <sheet name="Parça-İthal-Pompa-Civata" sheetId="69" r:id="rId42"/>
-    <sheet name="Parça-Hidros-Tank-Dikey" sheetId="36" r:id="rId43"/>
-    <sheet name="Parça-İthal-Tank-Dikey-Yatay" sheetId="70" r:id="rId44"/>
-    <sheet name="Parça-Hidros-Tank-Yatay" sheetId="37" r:id="rId45"/>
-    <sheet name="Parça-Hidros-Valf-Dikey-Esp_Gnl" sheetId="38" r:id="rId46"/>
-    <sheet name="Parça-İthal-Valf-Dikey-Esp_Gnl" sheetId="75" r:id="rId47"/>
-    <sheet name="Parça-Hidros-Valf-Dikey-EspÇift" sheetId="39" r:id="rId48"/>
-    <sheet name="Parça-İthal-Valf-Dikey-Esp-Hız" sheetId="76" r:id="rId49"/>
-    <sheet name="Parça-Yatay-Tank" sheetId="40" r:id="rId50"/>
-    <sheet name="Parça-Hidros-Platform-Dev+yürü" sheetId="43" r:id="rId51"/>
-    <sheet name="Parça-İthal-Platform-Dev + yürü" sheetId="74" r:id="rId52"/>
-    <sheet name="Parça-Hidros-Genel" sheetId="44" r:id="rId53"/>
-    <sheet name="Parça-Hid-İth-Özel-Tank-Dikey" sheetId="65" r:id="rId54"/>
-    <sheet name="Parça-Hidros-Özel-Tank-Yatık" sheetId="71" r:id="rId55"/>
-    <sheet name="Parça-İthal-Özel-Tank-Yatık" sheetId="73" r:id="rId56"/>
-    <sheet name="Parça-Hidros-1 - Valf-" sheetId="79" r:id="rId57"/>
-    <sheet name="Parça-ithal-1 - Valf" sheetId="81" r:id="rId58"/>
-    <sheet name="Parça-Hidros-2-Valf" sheetId="83" r:id="rId59"/>
+    <sheet name="Parça-Hidros-Pompa-Civata" sheetId="35" r:id="rId40"/>
+    <sheet name="Parça-İthal-Pompa" sheetId="68" r:id="rId41"/>
+    <sheet name="Parça-Hidros-Tank-Dikey" sheetId="36" r:id="rId42"/>
+    <sheet name="Parça-Hidros-Tank-Yatay" sheetId="37" r:id="rId43"/>
+    <sheet name="Parça-Hidros-Valf-Dikey-Esp_Gnl" sheetId="38" r:id="rId44"/>
+    <sheet name="Parça-Hidros-Valf-Dikey-EspÇift" sheetId="39" r:id="rId45"/>
+    <sheet name="Parça-Yatay-Tank" sheetId="40" r:id="rId46"/>
+    <sheet name="Parça-Hidros-Platform-Dev+yürü" sheetId="43" r:id="rId47"/>
+    <sheet name="Parça-Hidros-Genel" sheetId="44" r:id="rId48"/>
+    <sheet name="Parça-Hidros-Özel-Tank-Yatık" sheetId="71" r:id="rId49"/>
+    <sheet name="Parça-Hidros-1 - Valf-" sheetId="79" r:id="rId50"/>
+    <sheet name="Parça-Hidros-2-Valf" sheetId="83" r:id="rId51"/>
+    <sheet name="Parça-İthal-Pompa-Civata" sheetId="69" r:id="rId52"/>
+    <sheet name="Parça-İthal-Tank-Dikey-Yatay" sheetId="70" r:id="rId53"/>
+    <sheet name="Parça-İthal-Valf-Dikey-Esp_Gnl" sheetId="75" r:id="rId54"/>
+    <sheet name="Parça-İthal-Valf-Dikey-Esp-Hız" sheetId="76" r:id="rId55"/>
+    <sheet name="Parça-İthal-Platform-Dev + yürü" sheetId="74" r:id="rId56"/>
+    <sheet name="Parça-Hid-İth-Özel-Tank-Dikey" sheetId="65" r:id="rId57"/>
+    <sheet name="Parça-İthal-Özel-Tank-Yatık" sheetId="73" r:id="rId58"/>
+    <sheet name="Parça-ithal-1 - Valf" sheetId="81" r:id="rId59"/>
     <sheet name="Parça-İthal-2-Valf" sheetId="84" r:id="rId60"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
@@ -8064,7 +8064,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8202,10 +8202,144 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA31902F-0832-4108-8634-040D685C8A2A}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="53.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C2" t="s">
+        <v>536</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C3" t="s">
+        <v>537</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B4" t="s">
+        <v>419</v>
+      </c>
+      <c r="C4" t="s">
+        <v>538</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C5" t="s">
+        <v>539</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" t="s">
+        <v>540</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B7" t="s">
+        <v>422</v>
+      </c>
+      <c r="C7" t="s">
+        <v>541</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C8" t="s">
+        <v>542</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73DDBDB-720A-4259-B3B8-B6F156BF1F6F}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -8269,138 +8403,6 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA31902F-0832-4108-8634-040D685C8A2A}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="53.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="B2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C2" t="s">
-        <v>536</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="B3" t="s">
-        <v>418</v>
-      </c>
-      <c r="C3" t="s">
-        <v>537</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="B4" t="s">
-        <v>419</v>
-      </c>
-      <c r="C4" t="s">
-        <v>538</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="B5" t="s">
-        <v>420</v>
-      </c>
-      <c r="C5" t="s">
-        <v>539</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" t="s">
-        <v>421</v>
-      </c>
-      <c r="C6" t="s">
-        <v>540</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="B7" t="s">
-        <v>422</v>
-      </c>
-      <c r="C7" t="s">
-        <v>541</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>423</v>
-      </c>
-      <c r="C8" t="s">
-        <v>542</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8700,6 +8702,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8787,6 +8790,238 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB23081-6940-409B-B521-D25ED59C31AB}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D2" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D3" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D4" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D5" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D6" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D7" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D8" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="D9" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="D10" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="D11" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>559</v>
+      </c>
+      <c r="D12" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>559</v>
+      </c>
+      <c r="D13" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>560</v>
+      </c>
+      <c r="D14" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>560</v>
+      </c>
+      <c r="D15" s="23">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E2D47E-BD4B-4357-A0EF-508B5CB47490}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -8939,486 +9174,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB23081-6940-409B-B521-D25ED59C31AB}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D2" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D3" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D4" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D5" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D6" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D7" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D8" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>558</v>
-      </c>
-      <c r="D9" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>558</v>
-      </c>
-      <c r="D10" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>558</v>
-      </c>
-      <c r="D11" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>440</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>559</v>
-      </c>
-      <c r="D12" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>440</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>559</v>
-      </c>
-      <c r="D13" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>560</v>
-      </c>
-      <c r="D14" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>560</v>
-      </c>
-      <c r="D15" s="23">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F282FF6F-B057-4F3C-BA4B-3D8824148054}">
-  <dimension ref="A1:D19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D2" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D3" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D4" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D5" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D6" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D7" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D8" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>558</v>
-      </c>
-      <c r="D9" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>558</v>
-      </c>
-      <c r="D10" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>558</v>
-      </c>
-      <c r="D11" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>440</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>559</v>
-      </c>
-      <c r="D12" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>440</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>559</v>
-      </c>
-      <c r="D13" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>560</v>
-      </c>
-      <c r="D14" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>441</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>560</v>
-      </c>
-      <c r="D15" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
-        <v>519</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>594</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F657B9AA-C0EA-4266-8F38-BDA0BEAE883F}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9590,331 +9351,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75113117-3D3B-46BC-9E02-663CA120AA8D}">
-  <dimension ref="A1:N26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="47.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>523</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="E2" s="44" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
-        <v>525</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>392</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>393</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>526</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>398</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
-        <v>527</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="41" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>606</v>
-      </c>
-      <c r="D10" s="26">
-        <v>1</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="26" t="s">
-        <v>577</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>578</v>
-      </c>
-      <c r="D11" s="26">
-        <v>4</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="26" t="s">
-        <v>496</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>495</v>
-      </c>
-      <c r="D12" s="26">
-        <v>2</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="26" t="s">
-        <v>498</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="D13" s="26">
-        <v>2</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>602</v>
-      </c>
-      <c r="D14" s="26">
-        <v>4</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>603</v>
-      </c>
-      <c r="D15" s="26">
-        <v>4</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>609</v>
-      </c>
-      <c r="D16" s="47">
-        <v>4</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>602</v>
-      </c>
-      <c r="D17" s="26">
-        <v>4</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>603</v>
-      </c>
-      <c r="D18" s="26">
-        <v>4</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="E21" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CAAB65-5513-42C9-935D-0E8576F3E914}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10081,15 +9527,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A53901-52D0-4E8B-BDCC-705A28FC2A52}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10170,102 +9617,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31441649-E386-4460-A9D4-FEFE58B1EEA8}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B2" s="52"/>
-      <c r="C2" s="8" t="s">
-        <v>624</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>461</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>623</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="25" t="s">
-        <v>463</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>462</v>
-      </c>
-      <c r="D4" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="26" t="s">
-        <v>275</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="D5" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" s="53" t="s">
-        <v>492</v>
-      </c>
-      <c r="D6" s="32">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6DD818-438A-4831-92D3-0F7395A18832}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10380,129 +9741,445 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0619099-9FB9-4D8B-98C7-A6A2795A9397}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="67.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6552E6E-9DF3-44DF-85A1-A0D822031935}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
+        <v>477</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>478</v>
+      </c>
+      <c r="C2" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>480</v>
+      </c>
+      <c r="C3" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>481</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>482</v>
+      </c>
+      <c r="C4" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
+        <v>483</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>484</v>
+      </c>
+      <c r="C5" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="34" t="s">
+        <v>485</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
+        <v>486</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="C7" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="34" t="s">
+        <v>467</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>461</v>
+      </c>
+      <c r="C8" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
+        <v>468</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="C9" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="31" t="s">
+        <v>584</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>585</v>
+      </c>
+      <c r="C10" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="34" t="s">
+        <v>619</v>
+      </c>
+      <c r="B11" s="50"/>
+      <c r="C11" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="37" t="s">
+        <v>499</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="C12" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
+        <v>582</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>583</v>
+      </c>
+      <c r="C13" s="36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>494</v>
+      </c>
+      <c r="C14" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>472</v>
+      </c>
+      <c r="C15" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="34" t="s">
+        <v>586</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="C16" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="33" t="s">
+        <v>492</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" s="32">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB9543A-4A04-47DB-8957-17D1E7D8E982}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>491</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C856B513-77D9-4C37-8BCB-16B0C7D3D2BA}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD54F68-B6AB-4362-BF1C-5B9AF43B4B4B}">
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>442</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>416</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
-        <v>345</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>343</v>
-      </c>
-      <c r="C2" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
-        <v>580</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>579</v>
-      </c>
-      <c r="C3" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
-        <v>465</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="C4" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
-        <v>286</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>285</v>
-      </c>
-      <c r="C5" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
-        <v>493</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>494</v>
-      </c>
-      <c r="C6" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
-        <v>469</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>470</v>
-      </c>
-      <c r="C7" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
-        <v>471</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>472</v>
-      </c>
-      <c r="C8" s="32">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>578</v>
+      </c>
+      <c r="C2" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>593</v>
+      </c>
+      <c r="C3" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="B4" t="s">
+        <v>500</v>
+      </c>
+      <c r="C4" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="39"/>
+      <c r="B5" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="C5" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="24" t="s">
+        <v>598</v>
+      </c>
+      <c r="C6" s="26">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>474</v>
-      </c>
-      <c r="C9" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>625</v>
-      </c>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="24" t="s">
+        <v>596</v>
+      </c>
+      <c r="C7" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="26"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="26"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="26"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="26"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="26"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="26"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="26"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="26"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="26"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="26"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -10590,247 +10267,806 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0619099-9FB9-4D8B-98C7-A6A2795A9397}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F32166-8F4E-4DE8-B6BE-4D17E8330E25}">
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="67.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="9" max="9" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>442</v>
-      </c>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>581</v>
+        <v>600</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>617</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="60" t="s">
+        <v>628</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>486</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="D2" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="61"/>
+      <c r="B3" s="34" t="s">
+        <v>467</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>461</v>
+      </c>
+      <c r="D3" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="61"/>
+      <c r="B4" s="34" t="s">
+        <v>468</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="D4" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="61"/>
+      <c r="B5" s="33" t="s">
+        <v>492</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="61"/>
+      <c r="B6" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>480</v>
+      </c>
+      <c r="D6" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="61"/>
+      <c r="B7" s="34" t="s">
+        <v>626</v>
+      </c>
+      <c r="C7" s="51"/>
+      <c r="D7" s="36">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="61"/>
+      <c r="B8" s="34" t="s">
+        <v>637</v>
+      </c>
+      <c r="C8" s="51"/>
+      <c r="D8" s="36"/>
+      <c r="E8" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="61"/>
+      <c r="B9" s="34" t="s">
+        <v>632</v>
+      </c>
+      <c r="C9" s="45"/>
+      <c r="D9" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="61"/>
+      <c r="B10" s="34" t="s">
+        <v>582</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>583</v>
+      </c>
+      <c r="D10" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="61"/>
+      <c r="B11" s="37" t="s">
+        <v>499</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="D11" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="61"/>
+      <c r="B12" s="34" t="s">
+        <v>485</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="D12" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="61"/>
+      <c r="B13" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>472</v>
+      </c>
+      <c r="D13" s="36">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="61"/>
+      <c r="B14" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>494</v>
+      </c>
+      <c r="D14" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>629</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>486</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="D16" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="34" t="s">
+        <v>467</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>461</v>
+      </c>
+      <c r="D17" s="36">
+        <v>1</v>
+      </c>
+      <c r="I17" s="56"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="56"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="34" t="s">
+        <v>468</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="D18" s="36">
+        <v>1</v>
+      </c>
+      <c r="I18" s="56"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="56"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="33" t="s">
+        <v>492</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>480</v>
+      </c>
+      <c r="D20" s="36">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="34" t="s">
+        <v>481</v>
+      </c>
+      <c r="C21" s="51"/>
+      <c r="D21" s="36">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="34" t="s">
+        <v>639</v>
+      </c>
+      <c r="C22" s="51"/>
+      <c r="D22" s="36"/>
+      <c r="E22" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="34" t="s">
+        <v>627</v>
+      </c>
+      <c r="C23" s="45"/>
+      <c r="D23" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="34" t="s">
+        <v>582</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>583</v>
+      </c>
+      <c r="D24" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="31" t="s">
+        <v>584</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>585</v>
+      </c>
+      <c r="D25" s="36">
+        <v>1</v>
+      </c>
+      <c r="E25" s="54"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="34" t="s">
+        <v>586</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="D26" s="36">
+        <v>2</v>
+      </c>
+      <c r="E26" s="54"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="34" t="s">
+        <v>631</v>
+      </c>
+      <c r="C27" s="50"/>
+      <c r="D27" s="36">
+        <v>4</v>
+      </c>
+      <c r="E27" s="54"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="34" t="s">
+        <v>477</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>478</v>
+      </c>
+      <c r="D28" s="36">
+        <v>1</v>
+      </c>
+      <c r="E28" s="54"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="56"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="54"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>405</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>486</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="D30" s="36">
+        <v>1</v>
+      </c>
+      <c r="E30" s="55"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="56"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="34" t="s">
+        <v>467</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>461</v>
+      </c>
+      <c r="D31" s="36">
+        <v>1</v>
+      </c>
+      <c r="I31" s="56"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="56"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="34" t="s">
+        <v>468</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="D32" s="36">
+        <v>1</v>
+      </c>
+      <c r="I32" s="56"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="56"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="33" t="s">
+        <v>492</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="32">
+        <v>4</v>
+      </c>
+      <c r="I33" s="56"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="56"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>480</v>
+      </c>
+      <c r="D34" s="36">
+        <v>1</v>
+      </c>
+      <c r="I34" s="56"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="56"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" s="34" t="s">
+        <v>630</v>
+      </c>
+      <c r="C35" s="51"/>
+      <c r="D35" s="36">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>641</v>
+      </c>
+      <c r="I35" s="56"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="56"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B36" s="34" t="s">
+        <v>640</v>
+      </c>
+      <c r="C36" s="51"/>
+      <c r="D36" s="36"/>
+      <c r="E36" t="s">
+        <v>638</v>
+      </c>
+      <c r="I36" s="56"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="56"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37" s="34" t="s">
+        <v>627</v>
+      </c>
+      <c r="C37" s="45"/>
+      <c r="D37" s="36">
+        <v>3</v>
+      </c>
+      <c r="I37" s="56"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="56"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38" s="34" t="s">
+        <v>582</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>583</v>
+      </c>
+      <c r="D38" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="31" t="s">
+        <v>584</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>585</v>
+      </c>
+      <c r="D39" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B40" s="34" t="s">
+        <v>586</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="D40" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B41" s="34" t="s">
+        <v>631</v>
+      </c>
+      <c r="C41" s="50"/>
+      <c r="D41" s="36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B42" s="34" t="s">
+        <v>477</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>478</v>
+      </c>
+      <c r="D42" s="36">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6552E6E-9DF3-44DF-85A1-A0D822031935}">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA052F2E-EC86-4116-9E80-DCC7094C51DC}">
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>636</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>486</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="D3" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>635</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>467</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>461</v>
+      </c>
+      <c r="D4" s="36">
+        <v>1</v>
+      </c>
+      <c r="I4" s="56"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="56"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="34" t="s">
+        <v>468</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="D5" s="36">
+        <v>1</v>
+      </c>
+      <c r="I5" s="56"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="56"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="33" t="s">
+        <v>492</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>480</v>
+      </c>
+      <c r="D7" s="36">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="34" t="s">
+        <v>481</v>
+      </c>
+      <c r="C8" s="51"/>
+      <c r="D8" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="34" t="s">
+        <v>483</v>
+      </c>
+      <c r="C9" s="51"/>
+      <c r="D9" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="34" t="s">
+        <v>619</v>
+      </c>
+      <c r="C10" s="45"/>
+      <c r="D10" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="34" t="s">
+        <v>582</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>583</v>
+      </c>
+      <c r="D11" s="36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="31" t="s">
+        <v>584</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>585</v>
+      </c>
+      <c r="D12" s="36">
+        <v>1</v>
+      </c>
+      <c r="E12" s="54"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="34" t="s">
+        <v>586</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="D13" s="36">
+        <v>2</v>
+      </c>
+      <c r="E13" s="54"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="34" t="s">
+        <v>631</v>
+      </c>
+      <c r="C14" s="50"/>
+      <c r="D14" s="36">
+        <v>4</v>
+      </c>
+      <c r="E14" s="54"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="37" t="s">
+        <v>499</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="D15" s="36">
+        <v>1</v>
+      </c>
+      <c r="E15" s="54"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="34" t="s">
+        <v>485</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="D16" s="36">
+        <v>1</v>
+      </c>
+      <c r="E16" s="55"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="56"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>472</v>
+      </c>
+      <c r="D17" s="36">
+        <v>1</v>
+      </c>
+      <c r="I17" s="56"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="56"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>494</v>
+      </c>
+      <c r="D18" s="36">
+        <v>1</v>
+      </c>
+      <c r="I18" s="56"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="56"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="34" t="s">
         <v>477</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="C19" s="35" t="s">
         <v>478</v>
       </c>
-      <c r="C2" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
-        <v>479</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>480</v>
-      </c>
-      <c r="C3" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
-        <v>481</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>482</v>
-      </c>
-      <c r="C4" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>484</v>
-      </c>
-      <c r="C5" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
-        <v>485</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>283</v>
-      </c>
-      <c r="C6" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
-        <v>486</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>466</v>
-      </c>
-      <c r="C7" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
-        <v>467</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>461</v>
-      </c>
-      <c r="C8" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
-        <v>468</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>463</v>
-      </c>
-      <c r="C9" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
-        <v>584</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>585</v>
-      </c>
-      <c r="C10" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="34" t="s">
-        <v>619</v>
-      </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
-        <v>499</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>464</v>
-      </c>
-      <c r="C12" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
-        <v>582</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>583</v>
-      </c>
-      <c r="C13" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="34" t="s">
-        <v>493</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>494</v>
-      </c>
-      <c r="C14" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
-        <v>471</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>472</v>
-      </c>
-      <c r="C15" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
-        <v>586</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>322</v>
-      </c>
-      <c r="C16" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
-        <v>492</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C17" s="32">
-        <v>4</v>
-      </c>
+      <c r="D19" s="36">
+        <v>1</v>
+      </c>
+      <c r="I19" s="56"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="56"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="56"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="56"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="56"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="56"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="56"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="56"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="56"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="58"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="56"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="56"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="56"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="56"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10838,6 +11074,775 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F282FF6F-B057-4F3C-BA4B-3D8824148054}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D2" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D3" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D4" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D5" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D6" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D7" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D8" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="D9" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="D10" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="D11" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>559</v>
+      </c>
+      <c r="D12" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>559</v>
+      </c>
+      <c r="D13" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>560</v>
+      </c>
+      <c r="D14" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>560</v>
+      </c>
+      <c r="D15" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>519</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>594</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75113117-3D3B-46BC-9E02-663CA120AA8D}">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>525</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>392</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>526</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>527</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>606</v>
+      </c>
+      <c r="D10" s="26">
+        <v>1</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="26" t="s">
+        <v>577</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>578</v>
+      </c>
+      <c r="D11" s="26">
+        <v>4</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="26" t="s">
+        <v>496</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>495</v>
+      </c>
+      <c r="D12" s="26">
+        <v>2</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="26" t="s">
+        <v>498</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="D13" s="26">
+        <v>2</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="D14" s="26">
+        <v>4</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>603</v>
+      </c>
+      <c r="D15" s="26">
+        <v>4</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>609</v>
+      </c>
+      <c r="D16" s="47">
+        <v>4</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B17" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="D17" s="26">
+        <v>4</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B18" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>603</v>
+      </c>
+      <c r="D18" s="26">
+        <v>4</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31441649-E386-4460-A9D4-FEFE58B1EEA8}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="52"/>
+      <c r="C2" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>623</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="25" t="s">
+        <v>463</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>462</v>
+      </c>
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>492</v>
+      </c>
+      <c r="D6" s="32">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C856B513-77D9-4C37-8BCB-16B0C7D3D2BA}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
+        <v>345</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="C2" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
+        <v>580</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>579</v>
+      </c>
+      <c r="C3" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="33" t="s">
+        <v>465</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
+        <v>493</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>494</v>
+      </c>
+      <c r="C6" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="33" t="s">
+        <v>469</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>470</v>
+      </c>
+      <c r="C7" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
+        <v>471</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>472</v>
+      </c>
+      <c r="C8" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>474</v>
+      </c>
+      <c r="C9" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C314D1D5-FA39-40D9-A452-3A1FF8713F84}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -11033,45 +12038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB9543A-4A04-47DB-8957-17D1E7D8E982}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>491</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A55962E-4CA7-4F4D-92FB-4DA09E0DAE8F}">
   <dimension ref="A1:J18"/>
   <sheetViews>
@@ -11215,155 +12182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD54F68-B6AB-4362-BF1C-5B9AF43B4B4B}">
-  <dimension ref="A1:J18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>577</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>578</v>
-      </c>
-      <c r="C2" s="26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>593</v>
-      </c>
-      <c r="C3" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="B4" t="s">
-        <v>500</v>
-      </c>
-      <c r="C4" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="39"/>
-      <c r="B5" s="24" t="s">
-        <v>597</v>
-      </c>
-      <c r="C5" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="24" t="s">
-        <v>598</v>
-      </c>
-      <c r="C6" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="24" t="s">
-        <v>596</v>
-      </c>
-      <c r="C7" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="26"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="26"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="26"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="26"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="26"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="26"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="26"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="26"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="26"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="26"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="26"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="26"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3780F1-5D9C-4F40-BF47-BEA04C9E0808}">
   <dimension ref="A1:J18"/>
   <sheetViews>
@@ -11516,528 +12335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F32166-8F4E-4DE8-B6BE-4D17E8330E25}">
-  <dimension ref="A1:K42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
-        <v>628</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>486</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>466</v>
-      </c>
-      <c r="D2" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="61"/>
-      <c r="B3" s="34" t="s">
-        <v>467</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>461</v>
-      </c>
-      <c r="D3" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="61"/>
-      <c r="B4" s="34" t="s">
-        <v>468</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>463</v>
-      </c>
-      <c r="D4" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="61"/>
-      <c r="B5" s="33" t="s">
-        <v>492</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="61"/>
-      <c r="B6" s="34" t="s">
-        <v>479</v>
-      </c>
-      <c r="C6" s="35" t="s">
-        <v>480</v>
-      </c>
-      <c r="D6" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="61"/>
-      <c r="B7" s="34" t="s">
-        <v>626</v>
-      </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="36">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="61"/>
-      <c r="B8" s="34" t="s">
-        <v>637</v>
-      </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="36"/>
-      <c r="E8" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="61"/>
-      <c r="B9" s="34" t="s">
-        <v>632</v>
-      </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="61"/>
-      <c r="B10" s="34" t="s">
-        <v>582</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>583</v>
-      </c>
-      <c r="D10" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="61"/>
-      <c r="B11" s="37" t="s">
-        <v>499</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>464</v>
-      </c>
-      <c r="D11" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="61"/>
-      <c r="B12" s="34" t="s">
-        <v>485</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>283</v>
-      </c>
-      <c r="D12" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="61"/>
-      <c r="B13" s="34" t="s">
-        <v>471</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>472</v>
-      </c>
-      <c r="D13" s="36">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="61"/>
-      <c r="B14" s="34" t="s">
-        <v>493</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>494</v>
-      </c>
-      <c r="D14" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>629</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>486</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>466</v>
-      </c>
-      <c r="D16" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="34" t="s">
-        <v>467</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>461</v>
-      </c>
-      <c r="D17" s="36">
-        <v>1</v>
-      </c>
-      <c r="I17" s="56"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="56"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="34" t="s">
-        <v>468</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>463</v>
-      </c>
-      <c r="D18" s="36">
-        <v>1</v>
-      </c>
-      <c r="I18" s="56"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="56"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="33" t="s">
-        <v>492</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="D19" s="32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="34" t="s">
-        <v>479</v>
-      </c>
-      <c r="C20" s="35" t="s">
-        <v>480</v>
-      </c>
-      <c r="D20" s="36">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="34" t="s">
-        <v>481</v>
-      </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="36">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="34" t="s">
-        <v>639</v>
-      </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="36"/>
-      <c r="E22" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="34" t="s">
-        <v>627</v>
-      </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="34" t="s">
-        <v>582</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>583</v>
-      </c>
-      <c r="D24" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="31" t="s">
-        <v>584</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>585</v>
-      </c>
-      <c r="D25" s="36">
-        <v>1</v>
-      </c>
-      <c r="E25" s="54"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="34" t="s">
-        <v>586</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>322</v>
-      </c>
-      <c r="D26" s="36">
-        <v>2</v>
-      </c>
-      <c r="E26" s="54"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="34" t="s">
-        <v>631</v>
-      </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="36">
-        <v>4</v>
-      </c>
-      <c r="E27" s="54"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="C28" s="35" t="s">
-        <v>478</v>
-      </c>
-      <c r="D28" s="36">
-        <v>1</v>
-      </c>
-      <c r="E28" s="54"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="56"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="54"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>405</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>486</v>
-      </c>
-      <c r="C30" s="35" t="s">
-        <v>466</v>
-      </c>
-      <c r="D30" s="36">
-        <v>1</v>
-      </c>
-      <c r="E30" s="55"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="56"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="34" t="s">
-        <v>467</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>461</v>
-      </c>
-      <c r="D31" s="36">
-        <v>1</v>
-      </c>
-      <c r="I31" s="56"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="56"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="34" t="s">
-        <v>468</v>
-      </c>
-      <c r="C32" s="32" t="s">
-        <v>463</v>
-      </c>
-      <c r="D32" s="36">
-        <v>1</v>
-      </c>
-      <c r="I32" s="56"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="56"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="33" t="s">
-        <v>492</v>
-      </c>
-      <c r="C33" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="D33" s="32">
-        <v>4</v>
-      </c>
-      <c r="I33" s="56"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="56"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="34" t="s">
-        <v>479</v>
-      </c>
-      <c r="C34" s="35" t="s">
-        <v>480</v>
-      </c>
-      <c r="D34" s="36">
-        <v>1</v>
-      </c>
-      <c r="I34" s="56"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="56"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="34" t="s">
-        <v>630</v>
-      </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="36">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>641</v>
-      </c>
-      <c r="I35" s="56"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="56"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="34" t="s">
-        <v>640</v>
-      </c>
-      <c r="C36" s="51"/>
-      <c r="D36" s="36"/>
-      <c r="E36" t="s">
-        <v>638</v>
-      </c>
-      <c r="I36" s="56"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="56"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="34" t="s">
-        <v>627</v>
-      </c>
-      <c r="C37" s="45"/>
-      <c r="D37" s="36">
-        <v>3</v>
-      </c>
-      <c r="I37" s="56"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="56"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="34" t="s">
-        <v>582</v>
-      </c>
-      <c r="C38" s="32" t="s">
-        <v>583</v>
-      </c>
-      <c r="D38" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="31" t="s">
-        <v>584</v>
-      </c>
-      <c r="C39" s="32" t="s">
-        <v>585</v>
-      </c>
-      <c r="D39" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="34" t="s">
-        <v>586</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>322</v>
-      </c>
-      <c r="D40" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="34" t="s">
-        <v>631</v>
-      </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="C42" s="35" t="s">
-        <v>478</v>
-      </c>
-      <c r="D42" s="36">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A14"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85D83451-CCAB-4C7B-80F5-AACF432170AD}">
   <dimension ref="A1:K45"/>
   <sheetViews>
@@ -12575,291 +12873,6 @@
   <mergeCells count="1">
     <mergeCell ref="A2:A14"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA052F2E-EC86-4116-9E80-DCC7094C51DC}">
-  <dimension ref="A1:K26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>636</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>486</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>466</v>
-      </c>
-      <c r="D3" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>635</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>467</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>461</v>
-      </c>
-      <c r="D4" s="36">
-        <v>1</v>
-      </c>
-      <c r="I4" s="56"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="56"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="34" t="s">
-        <v>468</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>463</v>
-      </c>
-      <c r="D5" s="36">
-        <v>1</v>
-      </c>
-      <c r="I5" s="56"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="56"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="33" t="s">
-        <v>492</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="34" t="s">
-        <v>479</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>480</v>
-      </c>
-      <c r="D7" s="36">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="34" t="s">
-        <v>481</v>
-      </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="34" t="s">
-        <v>483</v>
-      </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="34" t="s">
-        <v>619</v>
-      </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="34" t="s">
-        <v>582</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>583</v>
-      </c>
-      <c r="D11" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="31" t="s">
-        <v>584</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>585</v>
-      </c>
-      <c r="D12" s="36">
-        <v>1</v>
-      </c>
-      <c r="E12" s="54"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="34" t="s">
-        <v>586</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>322</v>
-      </c>
-      <c r="D13" s="36">
-        <v>2</v>
-      </c>
-      <c r="E13" s="54"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="34" t="s">
-        <v>631</v>
-      </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="36">
-        <v>4</v>
-      </c>
-      <c r="E14" s="54"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="37" t="s">
-        <v>499</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>464</v>
-      </c>
-      <c r="D15" s="36">
-        <v>1</v>
-      </c>
-      <c r="E15" s="54"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="34" t="s">
-        <v>485</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>283</v>
-      </c>
-      <c r="D16" s="36">
-        <v>1</v>
-      </c>
-      <c r="E16" s="55"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="56"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="34" t="s">
-        <v>471</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>472</v>
-      </c>
-      <c r="D17" s="36">
-        <v>1</v>
-      </c>
-      <c r="I17" s="56"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="34" t="s">
-        <v>493</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>494</v>
-      </c>
-      <c r="D18" s="36">
-        <v>1</v>
-      </c>
-      <c r="I18" s="56"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="56"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>478</v>
-      </c>
-      <c r="D19" s="36">
-        <v>1</v>
-      </c>
-      <c r="I19" s="56"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="56"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="56"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="56"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="56"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="56"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="56"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="56"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="58"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="56"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="56"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="56"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="56"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="56"/>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>